<commit_message>
Revert "Merge branch 'sit' of https://bitbucket.airtel.africa/bitbucket/scm/qaaa/cs-portal-automation_selenium into feature/final_csp_1.15"
This reverts commit f259d5325094ab81cf2f9a02e5b6984a2bb3d898, reversing
changes made to c502d495e6a6e0e3bbb5d0d4a6ae191e773471e7.
</commit_message>
<xml_diff>
--- a/resources/excels/NE.xlsx
+++ b/resources/excels/NE.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="1" windowHeight="20280" windowWidth="35835" xWindow="0" yWindow="465"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
-    <sheet name="Priority" r:id="rId2" sheetId="10"/>
-    <sheet name="Headers" r:id="rId3" sheetId="11"/>
-    <sheet name="NFTRTickets-Reg" r:id="rId4" sheetId="15"/>
-    <sheet name="All NFTR codes" r:id="rId5" sheetId="22"/>
-    <sheet name="NFTRTickets-San" r:id="rId6" sheetId="3"/>
-    <sheet name="FTRTickets-Reg" r:id="rId7" sheetId="14"/>
-    <sheet name="All FTR codes" r:id="rId8" sheetId="23"/>
-    <sheet name="FTRTickets-San" r:id="rId9" sheetId="2"/>
-    <sheet name="UserManagement" r:id="rId10" sheetId="13"/>
-    <sheet name="PinnedTags" r:id="rId11" sheetId="5"/>
-    <sheet name="Ticket State" r:id="rId12" sheetId="6"/>
-    <sheet name="TemplateManagement" r:id="rId13" sheetId="16"/>
-    <sheet name="Ticket Transfer Rules" r:id="rId14" sheetId="17"/>
-    <sheet name="Authentication Policy" r:id="rId15" sheetId="18"/>
-    <sheet name="Action Tagging" r:id="rId16" sheetId="19"/>
-    <sheet name="State Queue Mapping" r:id="rId17" sheetId="20"/>
-    <sheet name="Transfer To Queue" r:id="rId18" sheetId="21"/>
-    <sheet name="QuestionAnswerKey" r:id="rId19" sheetId="24"/>
+    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Priority" sheetId="10" r:id="rId2"/>
+    <sheet name="Headers" sheetId="11" r:id="rId3"/>
+    <sheet name="NFTRTickets-Reg" sheetId="15" r:id="rId4"/>
+    <sheet name="All NFTR codes" sheetId="22" r:id="rId5"/>
+    <sheet name="NFTRTickets-San" sheetId="3" r:id="rId6"/>
+    <sheet name="FTRTickets-Reg" sheetId="14" r:id="rId7"/>
+    <sheet name="All FTR codes" sheetId="23" r:id="rId8"/>
+    <sheet name="FTRTickets-San" sheetId="2" r:id="rId9"/>
+    <sheet name="UserManagement" sheetId="13" r:id="rId10"/>
+    <sheet name="PinnedTags" sheetId="5" r:id="rId11"/>
+    <sheet name="Ticket State" sheetId="6" r:id="rId12"/>
+    <sheet name="TemplateManagement" sheetId="16" r:id="rId13"/>
+    <sheet name="Ticket Transfer Rules" sheetId="17" r:id="rId14"/>
+    <sheet name="Authentication Policy" sheetId="18" r:id="rId15"/>
+    <sheet name="Action Tagging" sheetId="19" r:id="rId16"/>
+    <sheet name="State Queue Mapping" sheetId="20" r:id="rId17"/>
+    <sheet name="Transfer To Queue" sheetId="21" r:id="rId18"/>
+    <sheet name="QuestionAnswerKey" sheetId="24" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'FTRTickets-Reg'!$A$1:$F$1</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'FTRTickets-San'!$A$1:$E$126</definedName>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">'NFTRTickets-Reg'!$A$1:$AB$1</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'NFTRTickets-San'!$A$1:$AB$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'FTRTickets-Reg'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'FTRTickets-San'!$A$1:$E$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NFTRTickets-Reg'!$A$1:$AB$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'NFTRTickets-San'!$A$1:$AB$72</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="387">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -1213,16 +1213,12 @@
   </si>
   <si>
     <t>FnF Indicator</t>
-  </si>
-  <si>
-    <t>010721000178</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1413,77 +1409,77 @@
     </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="6" numFmtId="0" xfId="2"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="3"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="3"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="4"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="9" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="5"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="4"/>
     <cellStyle name="Normal 4" xfId="3"/>
@@ -1502,7 +1498,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1515,7 +1511,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1534,12 +1530,12 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1582,12 +1578,12 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1630,12 +1626,12 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1678,12 +1674,12 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1716,10 +1712,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1754,7 +1750,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1806,7 +1802,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1917,21 +1913,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1948,7 +1944,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2000,14 +1996,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2016,11 +2012,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -2158,13 +2154,13 @@
       <c r="Q5" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2173,9 +2169,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="1" max="1" width="20.375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,12 +2356,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2410,15 +2406,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule dxfId="0" priority="2" type="duplicateValues"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -2430,9 +2426,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2490,13 +2486,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2505,8 +2501,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="15" width="30.875" collapsed="true"/>
-    <col min="2" max="16384" style="15" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="30.875" style="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,12 +2553,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2571,10 +2567,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="13.375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="37.25" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.75" collapsed="true"/>
+    <col min="2" max="2" width="13.375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.25" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2595,12 +2591,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2609,19 +2605,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.75" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="16" width="10.875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="16" width="11.5" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="16" width="10.125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="16" width="10.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="16" width="11.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="16" width="10.25" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="16" width="10.125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="16" width="10.5" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="16" width="11.625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="16" width="11.875" collapsed="true"/>
+    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.875" style="16" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5" style="16" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.125" style="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10" style="16" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11" style="16" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.25" style="16" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.125" style="16" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" style="16" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.625" style="16" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.875" style="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2699,12 +2695,12 @@
       <c r="M2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2713,15 +2709,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="7" width="18.75" collapsed="true"/>
-    <col min="2" max="2" style="7" width="9.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="7" width="11.0" collapsed="true"/>
-    <col min="4" max="6" style="7" width="9.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="7" width="14.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="7" width="14.875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="7" width="15.625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="7" width="21.75" collapsed="false"/>
-    <col min="11" max="16384" style="7" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="18.75" style="7" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9" style="7"/>
+    <col min="3" max="3" width="11" style="7" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9" style="7"/>
+    <col min="7" max="7" width="14" style="7" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="21.75" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2963,13 +2959,13 @@
       <c r="A15" s="28"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2978,11 +2974,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="18" width="19.25" collapsed="true"/>
-    <col min="2" max="2" style="18" width="9.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="18" width="13.875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="18" width="11.5" collapsed="true"/>
-    <col min="5" max="16384" style="18" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="19.25" style="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9" style="18" collapsed="1"/>
+    <col min="3" max="3" width="13.875" style="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5" style="18" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9" style="18" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -3020,7 +3016,7 @@
         <v>173</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>34</v>
       </c>
@@ -3041,7 +3037,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row ht="15.75" r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>346</v>
       </c>
@@ -3062,7 +3058,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
     </row>
-    <row ht="15.75" r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>347</v>
       </c>
@@ -3084,13 +3080,13 @@
       <c r="K4" s="17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3099,8 +3095,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.25" collapsed="true"/>
+    <col min="1" max="1" width="23.125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3148,13 +3144,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3163,9 +3159,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.75" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="25.25" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="61.125" collapsed="false"/>
+    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
+    <col min="3" max="3" width="61.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3328,13 +3324,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3343,7 +3339,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3382,12 +3378,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
@@ -3396,15 +3392,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3921,7 +3917,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row ht="47.25" r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>242</v>
       </c>
@@ -4056,48 +4052,48 @@
       <c r="M22" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18.95" r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -4278,13 +4274,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AB75"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4293,32 +4289,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18.95" r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -4498,46 +4494,46 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
+    <sheetView topLeftCell="AV1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="BH2" sqref="BH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18.95" r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -4774,31 +4770,28 @@
       <c r="BF2" t="s">
         <v>69</v>
       </c>
-      <c r="BG2" t="s">
-        <v>387</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.125" collapsed="true"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4823,13 +4816,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4859,24 +4852,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4917,6 +4910,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes After NG and NE Deployment
</commit_message>
<xml_diff>
--- a/resources/excels/NE.xlsx
+++ b/resources/excels/NE.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="1" windowHeight="20280" windowWidth="35835" xWindow="0" yWindow="465"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
-    <sheet name="Priority" r:id="rId2" sheetId="10"/>
-    <sheet name="Headers" r:id="rId3" sheetId="11"/>
-    <sheet name="NFTRTickets-Reg" r:id="rId4" sheetId="15"/>
-    <sheet name="All NFTR codes" r:id="rId5" sheetId="22"/>
-    <sheet name="NFTRTickets-San" r:id="rId6" sheetId="3"/>
-    <sheet name="FTRTickets-Reg" r:id="rId7" sheetId="14"/>
-    <sheet name="All FTR codes" r:id="rId8" sheetId="23"/>
-    <sheet name="FTRTickets-San" r:id="rId9" sheetId="2"/>
-    <sheet name="UserManagement" r:id="rId10" sheetId="13"/>
-    <sheet name="PinnedTags" r:id="rId11" sheetId="5"/>
-    <sheet name="Ticket State" r:id="rId12" sheetId="6"/>
-    <sheet name="TemplateManagement" r:id="rId13" sheetId="16"/>
-    <sheet name="Ticket Transfer Rules" r:id="rId14" sheetId="17"/>
-    <sheet name="Authentication Policy" r:id="rId15" sheetId="18"/>
-    <sheet name="Action Tagging" r:id="rId16" sheetId="19"/>
-    <sheet name="State Queue Mapping" r:id="rId17" sheetId="20"/>
-    <sheet name="Transfer To Queue" r:id="rId18" sheetId="21"/>
-    <sheet name="QuestionAnswerKey" r:id="rId19" sheetId="24"/>
+    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Priority" sheetId="10" r:id="rId2"/>
+    <sheet name="Headers" sheetId="11" r:id="rId3"/>
+    <sheet name="NFTRTickets-Reg" sheetId="15" r:id="rId4"/>
+    <sheet name="All NFTR codes" sheetId="22" r:id="rId5"/>
+    <sheet name="NFTRTickets-San" sheetId="3" r:id="rId6"/>
+    <sheet name="FTRTickets-Reg" sheetId="14" r:id="rId7"/>
+    <sheet name="All FTR codes" sheetId="23" r:id="rId8"/>
+    <sheet name="FTRTickets-San" sheetId="2" r:id="rId9"/>
+    <sheet name="UserManagement" sheetId="13" r:id="rId10"/>
+    <sheet name="PinnedTags" sheetId="5" r:id="rId11"/>
+    <sheet name="Ticket State" sheetId="6" r:id="rId12"/>
+    <sheet name="TemplateManagement" sheetId="16" r:id="rId13"/>
+    <sheet name="Ticket Transfer Rules" sheetId="17" r:id="rId14"/>
+    <sheet name="Authentication Policy" sheetId="18" r:id="rId15"/>
+    <sheet name="Action Tagging" sheetId="19" r:id="rId16"/>
+    <sheet name="State Queue Mapping" sheetId="20" r:id="rId17"/>
+    <sheet name="Transfer To Queue" sheetId="21" r:id="rId18"/>
+    <sheet name="QuestionAnswerKey" sheetId="24" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'FTRTickets-Reg'!$A$1:$F$1</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'FTRTickets-San'!$A$1:$E$126</definedName>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">'NFTRTickets-Reg'!$A$1:$AB$1</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'NFTRTickets-San'!$A$1:$AB$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'FTRTickets-Reg'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'FTRTickets-San'!$A$1:$E$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NFTRTickets-Reg'!$A$1:$AB$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'NFTRTickets-San'!$A$1:$AB$72</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="411">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -1216,14 +1216,82 @@
   </si>
   <si>
     <t>010721000178</t>
+  </si>
+  <si>
+    <t>ADD ON BUNDLE USAGE</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>ACCOUNT INFORMATION DETAIL</t>
+  </si>
+  <si>
+    <t>Date &amp; time</t>
+  </si>
+  <si>
+    <t>Reference No.</t>
+  </si>
+  <si>
+    <t>Bill Amount</t>
+  </si>
+  <si>
+    <t>Amount Received</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>LINKED MSISDN</t>
+  </si>
+  <si>
+    <t>MSISDN</t>
+  </si>
+  <si>
+    <t>SIM Number</t>
+  </si>
+  <si>
+    <t>GSM Service Activation Date</t>
+  </si>
+  <si>
+    <t>Line Type</t>
+  </si>
+  <si>
+    <t>Payment Level</t>
+  </si>
+  <si>
+    <t>GSM Status</t>
+  </si>
+  <si>
+    <t>Current Usage Limit</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>CUG</t>
+  </si>
+  <si>
+    <t>DND</t>
+  </si>
+  <si>
+    <t>Security Deposit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1301,6 +1369,11 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1C293B"/>
+      <name val="Tondo-regular"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1340,7 +1413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1411,79 +1484,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
+  <cellXfs count="41">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="6" numFmtId="0" xfId="2"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="3"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="3"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="4"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="9" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="5"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="4"/>
     <cellStyle name="Normal 4" xfId="3"/>
@@ -1502,7 +1596,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1515,7 +1609,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1534,12 +1628,12 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1582,12 +1676,12 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1630,12 +1724,12 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1678,12 +1772,12 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1716,10 +1810,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1754,7 +1848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1806,7 +1900,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1917,21 +2011,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1948,7 +2042,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2000,30 +2094,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -2076,7 +2170,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>2390495</v>
       </c>
@@ -2103,7 +2197,7 @@
       </c>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2388192</v>
       </c>
@@ -2121,7 +2215,7 @@
       </c>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>2390495</v>
       </c>
@@ -2139,7 +2233,7 @@
       </c>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>2394650</v>
       </c>
@@ -2158,27 +2252,27 @@
       <c r="Q5" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="1" max="1" width="20.375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
         <v>39</v>
       </c>
@@ -2189,7 +2283,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="33" t="s">
         <v>357</v>
       </c>
@@ -2200,7 +2294,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="33" t="s">
         <v>42</v>
       </c>
@@ -2211,7 +2305,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="33" t="s">
         <v>43</v>
       </c>
@@ -2222,7 +2316,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="33" t="s">
         <v>44</v>
       </c>
@@ -2233,7 +2327,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="33" t="s">
         <v>358</v>
       </c>
@@ -2244,7 +2338,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="33" t="s">
         <v>359</v>
       </c>
@@ -2255,7 +2349,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" s="33" t="s">
         <v>333</v>
       </c>
@@ -2263,7 +2357,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="B9" s="33" t="s">
         <v>334</v>
       </c>
@@ -2271,7 +2365,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10" s="33" t="s">
         <v>335</v>
       </c>
@@ -2279,7 +2373,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" s="33" t="s">
         <v>336</v>
       </c>
@@ -2287,7 +2381,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" s="33" t="s">
         <v>337</v>
       </c>
@@ -2295,7 +2389,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" s="33" t="s">
         <v>338</v>
       </c>
@@ -2303,7 +2397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" s="33" t="s">
         <v>339</v>
       </c>
@@ -2311,7 +2405,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" s="33" t="s">
         <v>340</v>
       </c>
@@ -2319,7 +2413,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" s="33" t="s">
         <v>341</v>
       </c>
@@ -2327,7 +2421,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="33" t="s">
         <v>342</v>
       </c>
@@ -2335,7 +2429,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="33" t="s">
         <v>343</v>
       </c>
@@ -2343,7 +2437,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" s="33" t="s">
         <v>344</v>
       </c>
@@ -2351,7 +2445,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" s="33" t="s">
         <v>345</v>
       </c>
@@ -2360,21 +2454,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -2391,7 +2485,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>67</v>
       </c>
@@ -2410,15 +2504,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule dxfId="0" priority="2" type="duplicateValues"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -2428,14 +2522,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>57</v>
       </c>
@@ -2446,7 +2540,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2454,7 +2548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2462,7 +2556,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2470,7 +2564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2478,7 +2572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2490,26 +2584,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="15" width="30.875" collapsed="true"/>
-    <col min="2" max="16384" style="15" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="30.875" style="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9" style="15" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="14" t="s">
         <v>118</v>
       </c>
@@ -2517,7 +2611,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="15" t="s">
         <v>120</v>
       </c>
@@ -2525,7 +2619,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="15" t="s">
         <v>122</v>
       </c>
@@ -2533,7 +2627,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="15" t="s">
         <v>124</v>
       </c>
@@ -2541,43 +2635,43 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="15" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="13.375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="37.25" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.75" collapsed="true"/>
+    <col min="2" max="2" width="13.375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.25" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>128</v>
       </c>
@@ -2595,36 +2689,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.75" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="16" width="10.875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="16" width="11.5" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="16" width="10.125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="16" width="10.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="16" width="11.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="16" width="10.25" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="16" width="10.125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="16" width="10.5" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="16" width="11.625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="16" width="11.875" collapsed="true"/>
+    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.875" style="16" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5" style="16" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.125" style="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10" style="16" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11" style="16" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.25" style="16" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.125" style="16" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" style="16" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.625" style="16" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.875" style="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -2665,7 +2759,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>374</v>
       </c>
@@ -2699,32 +2793,32 @@
       <c r="M2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="7" width="18.75" collapsed="true"/>
-    <col min="2" max="2" style="7" width="9.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="7" width="11.0" collapsed="true"/>
-    <col min="4" max="6" style="7" width="9.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="7" width="14.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="7" width="14.875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="7" width="15.625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="7" width="21.75" collapsed="false"/>
-    <col min="11" max="16384" style="7" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="18.75" style="7" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9" style="7"/>
+    <col min="3" max="3" width="11" style="7" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9" style="7"/>
+    <col min="7" max="7" width="14" style="7" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="21.75" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
         <v>153</v>
       </c>
@@ -2756,7 +2850,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>160</v>
       </c>
@@ -2776,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="9" t="s">
         <v>264</v>
       </c>
@@ -2796,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="9" t="s">
         <v>266</v>
       </c>
@@ -2812,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="9" t="s">
         <v>267</v>
       </c>
@@ -2828,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="9" t="s">
         <v>268</v>
       </c>
@@ -2844,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="9" t="s">
         <v>269</v>
       </c>
@@ -2860,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="9" t="s">
         <v>270</v>
       </c>
@@ -2876,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="9" t="s">
         <v>271</v>
       </c>
@@ -2892,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="9" t="s">
         <v>272</v>
       </c>
@@ -2908,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="9" t="s">
         <v>273</v>
       </c>
@@ -2924,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="9" t="s">
         <v>274</v>
       </c>
@@ -2940,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="9" t="s">
         <v>275</v>
       </c>
@@ -2956,36 +3050,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="28"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="28"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="18" width="19.25" collapsed="true"/>
-    <col min="2" max="2" style="18" width="9.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="18" width="13.875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="18" width="11.5" collapsed="true"/>
-    <col min="5" max="16384" style="18" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="19.25" style="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9" style="18" collapsed="1"/>
+    <col min="3" max="3" width="13.875" style="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5" style="18" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9" style="18" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>163</v>
       </c>
@@ -3020,7 +3114,7 @@
         <v>173</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="33" t="s">
         <v>34</v>
       </c>
@@ -3041,7 +3135,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row ht="15.75" r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="33" t="s">
         <v>346</v>
       </c>
@@ -3062,7 +3156,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
     </row>
-    <row ht="15.75" r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="33" t="s">
         <v>347</v>
       </c>
@@ -3084,26 +3178,26 @@
       <c r="K4" s="17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.25" collapsed="true"/>
+    <col min="1" max="1" width="23.125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>131</v>
       </c>
@@ -3114,7 +3208,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="33" t="s">
         <v>34</v>
       </c>
@@ -3125,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="33" t="s">
         <v>346</v>
       </c>
@@ -3136,7 +3230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="33" t="s">
         <v>347</v>
       </c>
@@ -3148,27 +3242,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.75" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="25.25" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="61.125" collapsed="false"/>
+    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
+    <col min="3" max="3" width="61.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>278</v>
       </c>
@@ -3179,7 +3273,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>279</v>
       </c>
@@ -3190,7 +3284,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>283</v>
       </c>
@@ -3201,7 +3295,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
@@ -3212,7 +3306,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>288</v>
       </c>
@@ -3223,7 +3317,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>291</v>
       </c>
@@ -3232,7 +3326,7 @@
       </c>
       <c r="C6" s="31"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>293</v>
       </c>
@@ -3243,7 +3337,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>296</v>
       </c>
@@ -3254,7 +3348,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>310</v>
       </c>
@@ -3265,7 +3359,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>311</v>
       </c>
@@ -3276,7 +3370,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>312</v>
       </c>
@@ -3287,7 +3381,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>314</v>
       </c>
@@ -3298,7 +3392,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>315</v>
       </c>
@@ -3307,7 +3401,7 @@
       </c>
       <c r="C13" s="31"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>313</v>
       </c>
@@ -3316,7 +3410,7 @@
       </c>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>316</v>
       </c>
@@ -3328,86 +3422,86 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>76</v>
       </c>
@@ -3448,7 +3542,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -3475,7 +3569,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
@@ -3502,7 +3596,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
@@ -3529,7 +3623,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
@@ -3562,7 +3656,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
@@ -3587,7 +3681,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>102</v>
       </c>
@@ -3612,7 +3706,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>104</v>
       </c>
@@ -3639,7 +3733,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
         <v>107</v>
       </c>
@@ -3666,7 +3760,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="23" t="s">
         <v>191</v>
       </c>
@@ -3693,7 +3787,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="23" t="s">
         <v>196</v>
       </c>
@@ -3720,7 +3814,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="23" t="s">
         <v>202</v>
       </c>
@@ -3751,7 +3845,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
         <v>210</v>
       </c>
@@ -3776,7 +3870,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="23" t="s">
         <v>215</v>
       </c>
@@ -3813,7 +3907,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="23" t="s">
         <v>220</v>
       </c>
@@ -3844,7 +3938,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="23" t="s">
         <v>223</v>
       </c>
@@ -3869,7 +3963,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="23" t="s">
         <v>227</v>
       </c>
@@ -3894,7 +3988,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="23" t="s">
         <v>237</v>
       </c>
@@ -3921,7 +4015,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row ht="47.25" r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="47.25">
       <c r="A19" s="23" t="s">
         <v>242</v>
       </c>
@@ -3962,7 +4056,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="23" t="s">
         <v>248</v>
       </c>
@@ -3991,7 +4085,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>375</v>
       </c>
@@ -4026,7 +4120,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
         <v>383</v>
       </c>
@@ -4055,49 +4149,133 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
+    <row r="23" spans="1:13" ht="16.5">
+      <c r="A23" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="39" t="s">
+        <v>399</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>405</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>406</v>
+      </c>
+      <c r="I25" s="40" t="s">
+        <v>407</v>
+      </c>
+      <c r="J25" s="40" t="s">
+        <v>408</v>
+      </c>
+      <c r="K25" s="40" t="s">
+        <v>409</v>
+      </c>
+      <c r="L25" s="40" t="s">
+        <v>410</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18.95" r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -4278,47 +4456,47 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AB75"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18.95" r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -4498,46 +4676,46 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
+    <sheetView topLeftCell="AV1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="BH2" sqref="BH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18.95" r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -4716,7 +4894,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59">
       <c r="A2" s="34" t="s">
         <v>365</v>
       </c>
@@ -4779,29 +4957,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.125" collapsed="true"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -4823,22 +5001,22 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -4859,27 +5037,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -4899,7 +5077,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="34" t="s">
         <v>360</v>
       </c>
@@ -4917,6 +5095,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>